<commit_message>
Can't export a full list of figures
</commit_message>
<xml_diff>
--- a/Output_Files/Sediment_Volume/pond_summary_sed_vol_102723.xlsx
+++ b/Output_Files/Sediment_Volume/pond_summary_sed_vol_102723.xlsx
@@ -1,21 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kag326\Documents\DEC_Ponds\Output_Files\Sediment_Volume\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8367119-172F-4975-9517-EA8AAEE229AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="660" yWindow="525" windowWidth="23310" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Pond_Name</t>
+  </si>
+  <si>
+    <t>TIN_mean_sed_depth</t>
+  </si>
+  <si>
+    <t>TIN_sed_volume</t>
+  </si>
+  <si>
+    <t>IDW_mean_sed_depth</t>
+  </si>
+  <si>
+    <t>IDW_sed_volume</t>
+  </si>
+  <si>
+    <t>SOAP_mean_sed_depth</t>
+  </si>
+  <si>
+    <t>SOAP_sed_volume</t>
+  </si>
+  <si>
+    <t>Boyce</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Howarth</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>Shelterbelt</t>
+  </si>
+  <si>
+    <t>Mt_Pleasant_SE</t>
+  </si>
+  <si>
+    <t>Harrison</t>
+  </si>
+  <si>
+    <t>Levine</t>
+  </si>
+  <si>
+    <t>Aquadro</t>
+  </si>
+  <si>
+    <t>Applegate</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +125,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +177,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +211,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +246,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,189 +422,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Pond_Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TIN_mean_sed_depth</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TIN_sed_volume</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>IDW_mean_sed_depth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>IDW_sed_volume</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SOAP_mean_sed_depth</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>SOAP_sed_volume</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Boyce</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>0.06419393274040326</v>
+        <v>6.4193932740403262E-2</v>
       </c>
       <c r="C2">
-        <v>368.9230967293464</v>
+        <v>368.92309672934641</v>
       </c>
       <c r="D2">
-        <v>0.05838948191990261</v>
+        <v>5.8389481919902612E-2</v>
       </c>
       <c r="E2">
-        <v>335.5648667518814</v>
+        <v>335.56486675188142</v>
       </c>
       <c r="F2">
-        <v>0.08666665475867254</v>
+        <v>8.6666654758672537E-2</v>
       </c>
       <c r="G2">
-        <v>498.0740280555954</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>White</t>
-        </is>
+        <v>498.07402805559542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>0.07017328299398283</v>
+        <v>7.017328299398283E-2</v>
       </c>
       <c r="C3">
-        <v>68.73912620827507</v>
+        <v>68.739126208275067</v>
       </c>
       <c r="D3">
-        <v>0.0583572716451758</v>
+        <v>5.8357271645175797E-2</v>
       </c>
       <c r="E3">
-        <v>57.16460296053557</v>
+        <v>57.164602960535568</v>
       </c>
       <c r="F3">
-        <v>0.09866279244317461</v>
+        <v>9.8662792443174607E-2</v>
       </c>
       <c r="G3">
-        <v>96.64638524028817</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Howarth</t>
-        </is>
+        <v>96.646385240288168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>0.08500830576505695</v>
+        <v>8.5008305765056955E-2</v>
       </c>
       <c r="C4">
-        <v>185.9787021889005</v>
+        <v>185.97870218890051</v>
       </c>
       <c r="D4">
-        <v>0.06928838410684041</v>
+        <v>6.9288384106840406E-2</v>
       </c>
       <c r="E4">
-        <v>151.5871141882365</v>
+        <v>151.58711418823651</v>
       </c>
       <c r="F4">
-        <v>0.1306867632039199</v>
+        <v>0.13068676320391989</v>
       </c>
       <c r="G4">
-        <v>285.912704590377</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Edwards</t>
-        </is>
+        <v>285.91270459037702</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0.1749721743104109</v>
       </c>
       <c r="C5">
-        <v>358.3786742295803</v>
+        <v>358.37867422958033</v>
       </c>
       <c r="D5">
         <v>0.1377091722688274</v>
       </c>
       <c r="E5">
-        <v>282.0564514412553</v>
+        <v>282.05645144125532</v>
       </c>
       <c r="F5">
-        <v>0.1985224784791189</v>
+        <v>0.19852247847911891</v>
       </c>
       <c r="G5">
-        <v>406.6144969765276</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Shelterbelt</t>
-        </is>
+        <v>406.61449697652762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>0.04448676498482714</v>
+        <v>4.4486764984827142E-2</v>
       </c>
       <c r="C6">
-        <v>45.7061792004659</v>
+        <v>45.706179200465897</v>
       </c>
       <c r="D6">
-        <v>0.03367558142920449</v>
+        <v>3.3675581429204487E-2</v>
       </c>
       <c r="E6">
-        <v>34.59865332999743</v>
+        <v>34.598653329997433</v>
       </c>
       <c r="F6">
-        <v>0.05999995930275797</v>
+        <v>5.999995930275797E-2</v>
       </c>
       <c r="G6">
-        <v>61.64460132913332</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Mt_Pleasant_SE</t>
-        </is>
+        <v>61.644601329133323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>0.08602332816963301</v>
+        <v>8.6023328169633012E-2</v>
       </c>
       <c r="C7">
-        <v>278.6111966466619</v>
+        <v>278.61119664666188</v>
       </c>
       <c r="D7">
-        <v>0.06686151681665174</v>
+        <v>6.6861516816651742E-2</v>
       </c>
       <c r="E7">
         <v>216.5501801228173</v>
@@ -541,101 +589,93 @@
         <v>0.1199950901292646</v>
       </c>
       <c r="G7">
-        <v>388.6384817233827</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Harrison</t>
-        </is>
+        <v>388.63848172338271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0.1249682586747079</v>
       </c>
       <c r="C8">
-        <v>189.2341259439355</v>
+        <v>189.23412594393551</v>
       </c>
       <c r="D8">
         <v>0.1074960810726979</v>
       </c>
       <c r="E8">
-        <v>162.7767495515833</v>
+        <v>162.77674955158329</v>
       </c>
       <c r="F8">
-        <v>0.14897457444245</v>
+        <v>0.14897457444244999</v>
       </c>
       <c r="G8">
         <v>225.5858702157968</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Levine</t>
-        </is>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>0.05050076710045913</v>
+        <v>5.0500767100459129E-2</v>
       </c>
       <c r="C9">
-        <v>99.75272038549009</v>
+        <v>99.752720385490093</v>
       </c>
       <c r="D9">
-        <v>0.03929011407620959</v>
+        <v>3.9290114076209588E-2</v>
       </c>
       <c r="E9">
-        <v>77.6086382125968</v>
+        <v>77.608638212596802</v>
       </c>
       <c r="F9">
-        <v>0.0631223013061715</v>
+        <v>6.3122301306171497E-2</v>
       </c>
       <c r="G9">
         <v>124.6836757896681</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Aquadro</t>
-        </is>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
       </c>
       <c r="B10">
         <v>0.1247033427336348</v>
       </c>
       <c r="C10">
-        <v>92.33727808750793</v>
+        <v>92.337278087507926</v>
       </c>
       <c r="D10">
-        <v>0.09323838731230273</v>
+        <v>9.3238387312302731E-2</v>
       </c>
       <c r="E10">
-        <v>69.03887826067678</v>
+        <v>69.038878260676782</v>
       </c>
       <c r="F10">
-        <v>0.1529721820199529</v>
+        <v>0.15297218201995291</v>
       </c>
       <c r="G10">
         <v>113.2690960899117</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Applegate</t>
-        </is>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>0.09238517900280177</v>
+        <v>9.2385179002801771E-2</v>
       </c>
       <c r="C11">
-        <v>908.8205026049631</v>
+        <v>908.82050260496305</v>
       </c>
       <c r="D11">
-        <v>0.05794195607563875</v>
+        <v>5.7941956075638748E-2</v>
       </c>
       <c r="E11">
-        <v>569.9922672767643</v>
+        <v>569.99226727676432</v>
       </c>
       <c r="F11">
         <v>0.109797818164223</v>
@@ -646,5 +686,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>